<commit_message>
refactor: update formated date import data
</commit_message>
<xml_diff>
--- a/public/excel/example_import_keuangan.xlsx
+++ b/public/excel/example_import_keuangan.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -80,15 +80,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="[$-421]dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,6 +112,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,7 +163,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,6 +173,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -191,10 +204,10 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.64"/>
@@ -202,9 +215,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -243,8 +256,8 @@
       <c r="B2" s="2" t="n">
         <v>45239</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>45239</v>
+      <c r="C2" s="3" t="n">
+        <v>45189</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>9</v>
@@ -272,8 +285,8 @@
       <c r="B3" s="2" t="n">
         <v>45239</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>45239</v>
+      <c r="C3" s="3" t="n">
+        <v>45189</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>12</v>
@@ -301,8 +314,8 @@
       <c r="B4" s="2" t="n">
         <v>45239</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>45239</v>
+      <c r="C4" s="3" t="n">
+        <v>45189</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>15</v>
@@ -319,15 +332,15 @@
       <c r="H4" s="0" t="n">
         <v>27823</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J8" s="3"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J9" s="3"/>
+      <c r="J9" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>